<commit_message>
update corona report excel manually (vacc data)
</commit_message>
<xml_diff>
--- a/data/kbvreport_export/faktenblatttabellen_2021-01-31.xlsx
+++ b/data/kbvreport_export/faktenblatttabellen_2021-01-31.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="343">
   <si>
     <t xml:space="preserve">Testungen</t>
   </si>
@@ -164,10 +164,10 @@
     <t xml:space="preserve">243</t>
   </si>
   <si>
-    <t xml:space="preserve">184</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-24,3 %</t>
+    <t xml:space="preserve">183</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-24,7 %</t>
   </si>
   <si>
     <t xml:space="preserve">Regionen mit 7-TI bei Über-60-Jährigen:</t>
@@ -390,10 +390,10 @@
     <t xml:space="preserve">80 Jahre +</t>
   </si>
   <si>
-    <t xml:space="preserve">3540 (19,0%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3502 (20,0%)</t>
+    <t xml:space="preserve">3539 (19,0%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3499 (20,0%)</t>
   </si>
   <si>
     <t xml:space="preserve"> -1,1%</t>
@@ -402,10 +402,10 @@
     <t xml:space="preserve">Gesamt</t>
   </si>
   <si>
-    <t xml:space="preserve">5005 ( 3,6%)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4796 ( 3,9%)</t>
+    <t xml:space="preserve">5004 ( 3,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4793 ( 3,9%)</t>
   </si>
   <si>
     <t xml:space="preserve"> -4,2%</t>
@@ -417,13 +417,37 @@
     <t xml:space="preserve">30 ( 1,8%)</t>
   </si>
   <si>
+    <t xml:space="preserve">80 ( 4,9%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">166,7%</t>
+  </si>
+  <si>
     <t xml:space="preserve">1011 (16,1%)</t>
   </si>
   <si>
+    <t xml:space="preserve">952 (15,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -5,8%</t>
+  </si>
+  <si>
     <t xml:space="preserve">5138 (47,9%)</t>
   </si>
   <si>
+    <t xml:space="preserve">4860 (45,3%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -5,4%</t>
+  </si>
+  <si>
     <t xml:space="preserve">6180 (33,2%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5892 (31,6%)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -4,7%</t>
   </si>
   <si>
     <t xml:space="preserve">Vorwarnzeit</t>
@@ -475,9 +499,15 @@
     <t xml:space="preserve">Bereits infizierte Bevölkerung</t>
   </si>
   <si>
+    <t xml:space="preserve">Inzidenzprojektion</t>
+  </si>
+  <si>
     <t xml:space="preserve">2,7 %</t>
   </si>
   <si>
+    <t xml:space="preserve">21.02.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Baden-Württemberg</t>
   </si>
   <si>
@@ -487,6 +517,9 @@
     <t xml:space="preserve">2,6 %</t>
   </si>
   <si>
+    <t xml:space="preserve">14.02.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bayern</t>
   </si>
   <si>
@@ -508,6 +541,9 @@
     <t xml:space="preserve">0,75</t>
   </si>
   <si>
+    <t xml:space="preserve">19.02.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bremen</t>
   </si>
   <si>
@@ -517,6 +553,9 @@
     <t xml:space="preserve">2,3 %</t>
   </si>
   <si>
+    <t xml:space="preserve">15.03.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hamburg</t>
   </si>
   <si>
@@ -526,9 +565,15 @@
     <t xml:space="preserve">2,5 %</t>
   </si>
   <si>
+    <t xml:space="preserve">11.04.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hessen</t>
   </si>
   <si>
+    <t xml:space="preserve">22.02.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Mecklenburg-Vorpommern</t>
   </si>
   <si>
@@ -547,21 +592,33 @@
     <t xml:space="preserve">1,8 %</t>
   </si>
   <si>
+    <t xml:space="preserve">24.02.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nordrhein-Westfalen</t>
   </si>
   <si>
+    <t xml:space="preserve">20.02.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Rheinland-Pfalz</t>
   </si>
   <si>
     <t xml:space="preserve">0,89</t>
   </si>
   <si>
+    <t xml:space="preserve">25.02.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Saarland</t>
   </si>
   <si>
     <t xml:space="preserve">0,98</t>
   </si>
   <si>
+    <t xml:space="preserve">19.09.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sachsen</t>
   </si>
   <si>
@@ -580,18 +637,27 @@
     <t xml:space="preserve">2,4 %</t>
   </si>
   <si>
+    <t xml:space="preserve">21.03.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Schleswig-Holstein</t>
   </si>
   <si>
     <t xml:space="preserve">1,02</t>
   </si>
   <si>
+    <t xml:space="preserve">nie</t>
+  </si>
+  <si>
     <t xml:space="preserve">Thüringen</t>
   </si>
   <si>
     <t xml:space="preserve">0,82</t>
   </si>
   <si>
+    <t xml:space="preserve">04.03.2021</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fälle gesamt</t>
   </si>
   <si>
@@ -727,10 +793,10 @@
     <t xml:space="preserve">Geimpfte Personen</t>
   </si>
   <si>
-    <t xml:space="preserve">Stand 26.1.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stand 2.2.</t>
+    <t xml:space="preserve">Stand 27.1.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stand 3.2.</t>
   </si>
   <si>
     <t xml:space="preserve">fdsa</t>
@@ -763,232 +829,235 @@
     <t xml:space="preserve">7-Tage-Inzidenz 80+</t>
   </si>
   <si>
-    <t xml:space="preserve">48,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,7</t>
+    <t xml:space="preserve">46,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56,6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18,5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41,7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,8</t>
   </si>
   <si>
     <t xml:space="preserve"> 3,5</t>
   </si>
   <si>
-    <t xml:space="preserve">1,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,5</t>
+    <t xml:space="preserve"> 0,6</t>
   </si>
   <si>
     <t xml:space="preserve">0,6</t>
   </si>
   <si>
-    <t xml:space="preserve">40,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,2</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">72,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 7,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1,1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,0</t>
+    <t xml:space="preserve">30,2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35,9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,1</t>
   </si>
   <si>
     <t xml:space="preserve">1,3</t>
   </si>
   <si>
-    <t xml:space="preserve">60,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 9,8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41,9</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 5,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 3,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 0,4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 8,0</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,2</t>
+    <t xml:space="preserve">63,8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10,4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4,9</t>
   </si>
   <si>
     <t xml:space="preserve">2,6</t>
   </si>
   <si>
-    <t xml:space="preserve">23,3</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 4,5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11,3</t>
+    <t xml:space="preserve">22,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6,1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11,7</t>
   </si>
 </sst>
 </file>
@@ -1420,34 +1489,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>236</v>
+        <v>258</v>
       </c>
       <c r="C1" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="D1" t="s">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="E1" t="s">
-        <v>239</v>
+        <v>261</v>
       </c>
       <c r="F1" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="G1" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="H1" t="s">
-        <v>242</v>
+        <v>264</v>
       </c>
       <c r="I1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="J1" t="s">
-        <v>243</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2">
@@ -1455,25 +1524,25 @@
         <v>124</v>
       </c>
       <c r="B2" t="s">
-        <v>244</v>
+        <v>266</v>
       </c>
       <c r="C2" t="s">
-        <v>245</v>
+        <v>267</v>
       </c>
       <c r="D2" t="s">
-        <v>246</v>
+        <v>268</v>
       </c>
       <c r="E2" t="s">
-        <v>247</v>
+        <v>269</v>
       </c>
       <c r="F2" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="G2" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="H2" t="n">
-        <v>2586997</v>
+        <v>2713210</v>
       </c>
       <c r="I2" t="n">
         <v>85</v>
@@ -1484,28 +1553,28 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>250</v>
+        <v>272</v>
       </c>
       <c r="C3" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="D3" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="E3" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="F3" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="G3" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="H3" t="n">
-        <v>308205</v>
+        <v>321814</v>
       </c>
       <c r="I3" t="n">
         <v>71</v>
@@ -1516,28 +1585,28 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>256</v>
+        <v>278</v>
       </c>
       <c r="C4" t="s">
-        <v>257</v>
+        <v>279</v>
       </c>
       <c r="D4" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="E4" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="F4" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="G4" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="H4" t="n">
-        <v>463122</v>
+        <v>484846</v>
       </c>
       <c r="I4" t="n">
         <v>84</v>
@@ -1548,28 +1617,28 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>261</v>
+        <v>282</v>
       </c>
       <c r="C5" t="s">
-        <v>262</v>
+        <v>283</v>
       </c>
       <c r="D5" t="s">
-        <v>263</v>
+        <v>284</v>
       </c>
       <c r="E5" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="F5" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="G5" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="H5" t="n">
-        <v>134937</v>
+        <v>140168</v>
       </c>
       <c r="I5" t="n">
         <v>75</v>
@@ -1580,28 +1649,28 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>267</v>
+        <v>288</v>
       </c>
       <c r="C6" t="s">
-        <v>253</v>
+        <v>289</v>
       </c>
       <c r="D6" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="E6" t="s">
-        <v>269</v>
+        <v>291</v>
       </c>
       <c r="F6" t="s">
-        <v>270</v>
+        <v>292</v>
       </c>
       <c r="G6" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="H6" t="n">
-        <v>89924</v>
+        <v>93555</v>
       </c>
       <c r="I6" t="n">
         <v>114</v>
@@ -1612,28 +1681,28 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>271</v>
+        <v>293</v>
       </c>
       <c r="C7" t="s">
-        <v>272</v>
+        <v>294</v>
       </c>
       <c r="D7" t="s">
-        <v>273</v>
+        <v>295</v>
       </c>
       <c r="E7" t="s">
-        <v>274</v>
+        <v>296</v>
       </c>
       <c r="F7" t="s">
-        <v>275</v>
+        <v>297</v>
       </c>
       <c r="G7" t="s">
-        <v>266</v>
+        <v>287</v>
       </c>
       <c r="H7" t="n">
-        <v>25682</v>
+        <v>26633</v>
       </c>
       <c r="I7" t="n">
         <v>89</v>
@@ -1644,28 +1713,28 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>276</v>
+        <v>298</v>
       </c>
       <c r="C8" t="s">
-        <v>277</v>
+        <v>299</v>
       </c>
       <c r="D8" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="E8" t="s">
-        <v>278</v>
+        <v>300</v>
       </c>
       <c r="F8" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="G8" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="H8" t="n">
-        <v>59820</v>
+        <v>63231</v>
       </c>
       <c r="I8" t="n">
         <v>70</v>
@@ -1676,28 +1745,28 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
-        <v>280</v>
+        <v>302</v>
       </c>
       <c r="C9" t="s">
-        <v>281</v>
+        <v>224</v>
       </c>
       <c r="D9" t="s">
-        <v>282</v>
+        <v>303</v>
       </c>
       <c r="E9" t="s">
-        <v>283</v>
+        <v>304</v>
       </c>
       <c r="F9" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="G9" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="H9" t="n">
-        <v>184555</v>
+        <v>190364</v>
       </c>
       <c r="I9" t="n">
         <v>88</v>
@@ -1708,28 +1777,28 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>286</v>
+        <v>306</v>
       </c>
       <c r="C10" t="s">
-        <v>287</v>
+        <v>267</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>307</v>
       </c>
       <c r="E10" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="F10" t="s">
-        <v>290</v>
+        <v>309</v>
       </c>
       <c r="G10" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="H10" t="n">
-        <v>73909</v>
+        <v>75926</v>
       </c>
       <c r="I10" t="n">
         <v>81</v>
@@ -1740,28 +1809,28 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="B11" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C11" t="s">
-        <v>292</v>
+        <v>311</v>
       </c>
       <c r="D11" t="s">
-        <v>293</v>
+        <v>312</v>
       </c>
       <c r="E11" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
       <c r="F11" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="G11" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="H11" t="n">
-        <v>208258</v>
+        <v>220200</v>
       </c>
       <c r="I11" t="n">
         <v>73</v>
@@ -1772,28 +1841,28 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>296</v>
+        <v>315</v>
       </c>
       <c r="C12" t="s">
-        <v>272</v>
+        <v>316</v>
       </c>
       <c r="D12" t="s">
-        <v>297</v>
+        <v>317</v>
       </c>
       <c r="E12" t="s">
-        <v>298</v>
+        <v>318</v>
       </c>
       <c r="F12" t="s">
-        <v>284</v>
+        <v>305</v>
       </c>
       <c r="G12" t="s">
-        <v>249</v>
+        <v>271</v>
       </c>
       <c r="H12" t="n">
-        <v>482207</v>
+        <v>514191</v>
       </c>
       <c r="I12" t="n">
         <v>81</v>
@@ -1804,28 +1873,28 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s">
-        <v>299</v>
+        <v>319</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
+        <v>320</v>
       </c>
       <c r="D13" t="s">
-        <v>268</v>
+        <v>321</v>
       </c>
       <c r="E13" t="s">
-        <v>300</v>
+        <v>322</v>
       </c>
       <c r="F13" t="s">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="G13" t="s">
-        <v>255</v>
+        <v>277</v>
       </c>
       <c r="H13" t="n">
-        <v>166064</v>
+        <v>172753</v>
       </c>
       <c r="I13" t="n">
         <v>74</v>
@@ -1836,28 +1905,28 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>302</v>
+        <v>324</v>
       </c>
       <c r="C14" t="s">
-        <v>303</v>
+        <v>325</v>
       </c>
       <c r="D14" t="s">
-        <v>304</v>
+        <v>248</v>
       </c>
       <c r="E14" t="s">
-        <v>305</v>
+        <v>240</v>
       </c>
       <c r="F14" t="s">
-        <v>295</v>
+        <v>314</v>
       </c>
       <c r="G14" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="H14" t="n">
-        <v>31961</v>
+        <v>33532</v>
       </c>
       <c r="I14" t="n">
         <v>115</v>
@@ -1868,28 +1937,28 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="C15" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="D15" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="E15" t="s">
-        <v>309</v>
+        <v>329</v>
       </c>
       <c r="F15" t="s">
-        <v>265</v>
+        <v>286</v>
       </c>
       <c r="G15" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="H15" t="n">
-        <v>112217</v>
+        <v>119455</v>
       </c>
       <c r="I15" t="n">
         <v>107</v>
@@ -1900,28 +1969,28 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
-        <v>311</v>
+        <v>331</v>
       </c>
       <c r="C16" t="s">
-        <v>312</v>
+        <v>332</v>
       </c>
       <c r="D16" t="s">
-        <v>228</v>
+        <v>252</v>
       </c>
       <c r="E16" t="s">
-        <v>278</v>
+        <v>333</v>
       </c>
       <c r="F16" t="s">
-        <v>284</v>
+        <v>334</v>
       </c>
       <c r="G16" t="s">
-        <v>260</v>
+        <v>281</v>
       </c>
       <c r="H16" t="n">
-        <v>73687</v>
+        <v>76834</v>
       </c>
       <c r="I16" t="n">
         <v>135</v>
@@ -1932,28 +2001,28 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>313</v>
+        <v>335</v>
       </c>
       <c r="C17" t="s">
-        <v>314</v>
+        <v>336</v>
       </c>
       <c r="D17" t="s">
-        <v>246</v>
+        <v>337</v>
       </c>
       <c r="E17" t="s">
-        <v>315</v>
+        <v>338</v>
       </c>
       <c r="F17" t="s">
-        <v>316</v>
+        <v>339</v>
       </c>
       <c r="G17" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="H17" t="n">
-        <v>106077</v>
+        <v>109776</v>
       </c>
       <c r="I17" t="n">
         <v>72</v>
@@ -1964,28 +2033,28 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="B18" t="s">
-        <v>317</v>
+        <v>340</v>
       </c>
       <c r="C18" t="s">
-        <v>318</v>
+        <v>341</v>
       </c>
       <c r="D18" t="s">
-        <v>319</v>
+        <v>342</v>
       </c>
       <c r="E18" t="s">
-        <v>269</v>
+        <v>308</v>
       </c>
       <c r="F18" t="s">
-        <v>275</v>
+        <v>297</v>
       </c>
       <c r="G18" t="s">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="H18" t="n">
-        <v>66372</v>
+        <v>69932</v>
       </c>
       <c r="I18" t="n">
         <v>152</v>
@@ -2501,38 +2570,54 @@
       <c r="B7" t="s">
         <v>129</v>
       </c>
-      <c r="C7"/>
-      <c r="D7"/>
+      <c r="C7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
         <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8"/>
-      <c r="D8"/>
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D8" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
         <v>120</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9"/>
-      <c r="D9"/>
+        <v>135</v>
+      </c>
+      <c r="C9" t="s">
+        <v>136</v>
+      </c>
+      <c r="D9" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
         <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10"/>
+        <v>138</v>
+      </c>
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" t="s">
+        <v>140</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2550,7 +2635,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -2564,13 +2649,13 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="D2" t="n">
         <v>8</v>
@@ -2578,13 +2663,13 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
@@ -2592,13 +2677,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="C4" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="D4" t="n">
         <v>-1</v>
@@ -2620,22 +2705,25 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="D1" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="E1" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="F1" t="s">
-        <v>147</v>
+        <v>155</v>
+      </c>
+      <c r="G1" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="2">
@@ -2655,15 +2743,18 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>157</v>
+      </c>
+      <c r="G2" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C3" t="n">
         <v>77</v>
@@ -2675,12 +2766,15 @@
         <v>35</v>
       </c>
       <c r="F3" t="s">
-        <v>151</v>
+        <v>161</v>
+      </c>
+      <c r="G3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
         <v>27</v>
@@ -2695,15 +2789,18 @@
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>153</v>
+        <v>164</v>
+      </c>
+      <c r="G4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>154</v>
+        <v>165</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
       <c r="C5" t="n">
         <v>87</v>
@@ -2715,15 +2812,18 @@
         <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>156</v>
+        <v>167</v>
+      </c>
+      <c r="G5" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C6" t="n">
         <v>130</v>
@@ -2735,15 +2835,18 @@
         <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>148</v>
+        <v>157</v>
+      </c>
+      <c r="G6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>172</v>
       </c>
       <c r="C7" t="n">
         <v>83</v>
@@ -2755,15 +2858,18 @@
         <v>41</v>
       </c>
       <c r="F7" t="s">
-        <v>161</v>
+        <v>173</v>
+      </c>
+      <c r="G7" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="B8" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="C8" t="n">
         <v>87</v>
@@ -2775,12 +2881,15 @@
         <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>164</v>
+        <v>177</v>
+      </c>
+      <c r="G8" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="B9" t="s">
         <v>26</v>
@@ -2795,15 +2904,18 @@
         <v>31</v>
       </c>
       <c r="F9" t="s">
-        <v>148</v>
+        <v>157</v>
+      </c>
+      <c r="G9" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>166</v>
+        <v>181</v>
       </c>
       <c r="B10" t="s">
-        <v>167</v>
+        <v>182</v>
       </c>
       <c r="C10" t="n">
         <v>91</v>
@@ -2815,15 +2927,18 @@
         <v>37</v>
       </c>
       <c r="F10" t="s">
-        <v>168</v>
+        <v>183</v>
+      </c>
+      <c r="G10" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="B11" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="C11" t="n">
         <v>79</v>
@@ -2835,12 +2950,15 @@
         <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>171</v>
+        <v>186</v>
+      </c>
+      <c r="G11" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>172</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
         <v>26</v>
@@ -2855,15 +2973,18 @@
         <v>35</v>
       </c>
       <c r="F12" t="s">
-        <v>148</v>
+        <v>157</v>
+      </c>
+      <c r="G12" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B13" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C13" t="n">
         <v>85</v>
@@ -2875,15 +2996,18 @@
         <v>36</v>
       </c>
       <c r="F13" t="s">
-        <v>161</v>
+        <v>173</v>
+      </c>
+      <c r="G13" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>176</v>
+        <v>194</v>
       </c>
       <c r="C14" t="n">
         <v>126</v>
@@ -2895,15 +3019,18 @@
         <v>46</v>
       </c>
       <c r="F14" t="s">
-        <v>151</v>
+        <v>161</v>
+      </c>
+      <c r="G14" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>177</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>178</v>
+        <v>197</v>
       </c>
       <c r="C15" t="n">
         <v>129</v>
@@ -2915,15 +3042,18 @@
         <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>179</v>
+        <v>198</v>
+      </c>
+      <c r="G15" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>180</v>
+        <v>199</v>
       </c>
       <c r="B16" t="s">
-        <v>181</v>
+        <v>200</v>
       </c>
       <c r="C16" t="n">
         <v>167</v>
@@ -2935,15 +3065,18 @@
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>182</v>
+        <v>201</v>
+      </c>
+      <c r="G16" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>203</v>
       </c>
       <c r="B17" t="s">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C17" t="n">
         <v>81</v>
@@ -2955,15 +3088,18 @@
         <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>168</v>
+        <v>183</v>
+      </c>
+      <c r="G17" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>185</v>
+        <v>206</v>
       </c>
       <c r="B18" t="s">
-        <v>186</v>
+        <v>207</v>
       </c>
       <c r="C18" t="n">
         <v>163</v>
@@ -2975,7 +3111,10 @@
         <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>153</v>
+        <v>164</v>
+      </c>
+      <c r="G18" t="s">
+        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -2994,354 +3133,354 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>187</v>
+        <v>209</v>
       </c>
       <c r="B1" t="s">
-        <v>188</v>
+        <v>210</v>
       </c>
       <c r="C1" t="s">
-        <v>189</v>
+        <v>211</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
+        <v>212</v>
       </c>
       <c r="E1" t="s">
-        <v>191</v>
+        <v>213</v>
       </c>
       <c r="F1" t="s">
-        <v>192</v>
+        <v>214</v>
       </c>
       <c r="G1" t="s">
-        <v>193</v>
+        <v>215</v>
       </c>
       <c r="H1" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="I1" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="J1" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="B2" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="C2" t="n">
         <v>984774</v>
       </c>
       <c r="D2" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="E2" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="F2" t="n">
         <v>88516</v>
       </c>
       <c r="G2" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="H2" t="n">
         <v>1669</v>
       </c>
       <c r="I2" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="J2" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="C3" t="n">
         <v>720516</v>
       </c>
       <c r="D3" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="E3" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="F3" t="n">
         <v>106367</v>
       </c>
       <c r="G3" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="H3" t="n">
         <v>1050</v>
       </c>
       <c r="I3" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="J3" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>230</v>
       </c>
       <c r="C4" t="n">
         <v>2743119</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="E4" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="F4" t="n">
         <v>57163</v>
       </c>
       <c r="G4" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="H4" t="n">
         <v>894</v>
       </c>
       <c r="I4" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="J4" t="s">
-        <v>210</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>234</v>
       </c>
       <c r="C5" t="n">
         <v>992075</v>
       </c>
       <c r="D5" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="E5" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="F5" t="n">
         <v>18335</v>
       </c>
       <c r="G5" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="H5" t="n">
         <v>626</v>
       </c>
       <c r="I5" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="J5" t="s">
-        <v>214</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>215</v>
+        <v>237</v>
       </c>
       <c r="C6" t="n">
         <v>3828183</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="F6" t="n">
         <v>37180</v>
       </c>
       <c r="G6" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="H6" t="n">
         <v>440</v>
       </c>
       <c r="I6" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="J6" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="B7" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="C7" t="n">
         <v>3255920</v>
       </c>
       <c r="D7" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="E7" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="F7" t="n">
         <v>76201</v>
       </c>
       <c r="G7" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="H7" t="n">
         <v>390</v>
       </c>
       <c r="I7" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="J7" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="B8" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="C8" t="n">
         <v>2553032</v>
       </c>
       <c r="D8" t="s">
-        <v>206</v>
+        <v>228</v>
       </c>
       <c r="E8" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="F8" t="n">
         <v>58319</v>
       </c>
       <c r="G8" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="H8" t="n">
         <v>284</v>
       </c>
       <c r="I8" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="J8" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="B9" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="C9" t="n">
         <v>1513385</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="E9" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="F9" t="n">
         <v>12482</v>
       </c>
       <c r="G9" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="H9" t="n">
         <v>210</v>
       </c>
       <c r="I9" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="J9" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="B10" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="C10" t="n">
         <v>728743</v>
       </c>
       <c r="D10" t="s">
-        <v>197</v>
+        <v>219</v>
       </c>
       <c r="E10" t="s">
-        <v>225</v>
+        <v>247</v>
       </c>
       <c r="F10" t="n">
         <v>16308</v>
       </c>
       <c r="G10" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="H10" t="n">
         <v>205</v>
       </c>
       <c r="I10" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="J10" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="C11" t="n">
         <v>2225659</v>
       </c>
       <c r="D11" t="s">
-        <v>211</v>
+        <v>233</v>
       </c>
       <c r="E11" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="F11" t="n">
         <v>14108</v>
       </c>
       <c r="G11" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="H11" t="n">
         <v>181</v>
       </c>
       <c r="I11" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="J11" t="s">
-        <v>230</v>
+        <v>252</v>
       </c>
     </row>
   </sheetData>
@@ -3360,24 +3499,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>231</v>
+        <v>253</v>
       </c>
       <c r="B1" t="s">
-        <v>232</v>
+        <v>254</v>
       </c>
       <c r="C1" t="s">
-        <v>233</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>234</v>
+        <v>256</v>
       </c>
       <c r="B2" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
       <c r="C2" t="s">
-        <v>235</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>